<commit_message>
(bug):export all student timetable
</commit_message>
<xml_diff>
--- a/student_timetable/5678_timetable.xlsx
+++ b/student_timetable/5678_timetable.xlsx
@@ -624,12 +624,12 @@
       </c>
       <c r="B10" s="6" t="inlineStr">
         <is>
-          <t>4:00 to 5:00(L + T)</t>
+          <t>4:00 to 5:00 (L + T)</t>
         </is>
       </c>
       <c r="C10" s="6" t="inlineStr">
         <is>
-          <t>MITS5003-(1h Lecture 1)</t>
+          <t>MITS5003- (1h Lecture 1)</t>
         </is>
       </c>
       <c r="D10" s="6" t="inlineStr">
@@ -657,12 +657,12 @@
       </c>
       <c r="B11" s="6" t="inlineStr">
         <is>
-          <t>14:00 to 15:00(L + T)</t>
+          <t>14:00 to 15:00 (L + T)</t>
         </is>
       </c>
       <c r="C11" s="6" t="inlineStr">
         <is>
-          <t>MITS5001-(1h Lecture 1)</t>
+          <t>MITS5001- (1h Lecture 1)</t>
         </is>
       </c>
       <c r="D11" s="6" t="inlineStr">
@@ -690,12 +690,12 @@
       </c>
       <c r="B12" s="6" t="inlineStr">
         <is>
-          <t>22:00 to 22:45(L + T)</t>
+          <t>22:00 to 22:45 (L + T)</t>
         </is>
       </c>
       <c r="C12" s="6" t="inlineStr">
         <is>
-          <t>MITS4003-(0h45min Lecture 2)</t>
+          <t>MITS4003- (0h45min Lecture 2)</t>
         </is>
       </c>
       <c r="D12" s="6" t="inlineStr">
@@ -723,12 +723,12 @@
       </c>
       <c r="B13" s="6" t="inlineStr">
         <is>
-          <t>22:00 to 22:45(L + T)</t>
+          <t>22:00 to 22:45 (L + T)</t>
         </is>
       </c>
       <c r="C13" s="6" t="inlineStr">
         <is>
-          <t>MITS4003-(0h45min Lecture 1)</t>
+          <t>MITS4003- (0h45min Lecture 1)</t>
         </is>
       </c>
       <c r="D13" s="6" t="inlineStr">
@@ -756,12 +756,12 @@
       </c>
       <c r="B14" s="6" t="inlineStr">
         <is>
-          <t>17:00 to 18:00(L + T)</t>
+          <t>17:00 to 18:00 (L + T)</t>
         </is>
       </c>
       <c r="C14" s="6" t="inlineStr">
         <is>
-          <t>MITS5001-(1h Tutorial 1)</t>
+          <t>MITS5001- (1h Tutorial 1)</t>
         </is>
       </c>
       <c r="D14" s="6" t="inlineStr">
@@ -789,12 +789,12 @@
       </c>
       <c r="B15" s="6" t="inlineStr">
         <is>
-          <t>22:00 to 22:30(L + T)</t>
+          <t>22:00 to 22:30 (L + T)</t>
         </is>
       </c>
       <c r="C15" s="6" t="inlineStr">
         <is>
-          <t>MITS5002-(0h30min Tutorial 1)</t>
+          <t>MITS5002- (0h30min Tutorial 1)</t>
         </is>
       </c>
       <c r="D15" s="6" t="inlineStr">
@@ -822,17 +822,17 @@
       </c>
       <c r="B16" s="6" t="inlineStr">
         <is>
-          <t>8:00 to 9:00(L + T)</t>
+          <t>7:00 to 8:00 (L + T)</t>
         </is>
       </c>
       <c r="C16" s="6" t="inlineStr">
         <is>
-          <t>MITS5003-(1h Tutorial 1)</t>
+          <t>MITS5003- (1h Tutorial 1)</t>
         </is>
       </c>
       <c r="D16" s="6" t="inlineStr">
         <is>
-          <t>65432</t>
+          <t>234</t>
         </is>
       </c>
       <c r="E16" s="6" t="n">
@@ -855,12 +855,12 @@
       </c>
       <c r="B17" s="6" t="inlineStr">
         <is>
-          <t>10:00 to 11:00(L + T)</t>
+          <t>10:00 to 11:00 (L + T)</t>
         </is>
       </c>
       <c r="C17" s="6" t="inlineStr">
         <is>
-          <t>MITS5002-(1h Lecture 1)</t>
+          <t>MITS5002- (1h Lecture 1)</t>
         </is>
       </c>
       <c r="D17" s="6" t="inlineStr">

</xml_diff>